<commit_message>
Updated results and front-end node
</commit_message>
<xml_diff>
--- a/LidarTestResults/dirtyRectangle.xlsx
+++ b/LidarTestResults/dirtyRectangle.xlsx
@@ -17,6 +17,10 @@
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -581,7 +585,7 @@
           <c:yMode val="edge"/>
           <c:x val="2.8170652782524598E-2"/>
           <c:y val="7.4977632123279347E-2"/>
-          <c:w val="0.6686252993381463"/>
+          <c:w val="0.82833226615903777"/>
           <c:h val="0.90278580941470732"/>
         </c:manualLayout>
       </c:layout>
@@ -2831,22 +2835,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>418.16321624972926</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>-88.378860391234937</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>-508.37370784517645</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>126.97158023829095</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>46.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>-25.808872000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2864,22 +2868,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>152.19896377992256</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>272.00216366041394</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>-185.03289753918673</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>-368.75224448373359</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>52.05</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>-64.792016000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2900,11 +2904,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="199703272"/>
-        <c:axId val="199703664"/>
+        <c:axId val="383356368"/>
+        <c:axId val="383356760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="199703272"/>
+        <c:axId val="383356368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2961,12 +2965,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199703664"/>
+        <c:crossAx val="383356760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="199703664"/>
+        <c:axId val="383356760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3023,7 +3027,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199703272"/>
+        <c:crossAx val="383356368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3927,7 +3931,7 @@
   <dimension ref="A1:I361"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3964,18 +3968,18 @@
         <v>8.2200834319605338</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>445</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H2">
         <f t="shared" ref="H2" si="2">F2*COS(G2*PI()/180)</f>
-        <v>0</v>
+        <v>418.16321624972926</v>
       </c>
       <c r="I2">
         <f t="shared" ref="I2" si="3">F2*SIN(G2*PI()/180)</f>
-        <v>0</v>
+        <v>152.19896377992256</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3993,13 +3997,19 @@
         <f t="shared" si="1"/>
         <v>16.332964456770455</v>
       </c>
+      <c r="F3">
+        <v>286</v>
+      </c>
+      <c r="G3">
+        <v>108</v>
+      </c>
       <c r="H3">
-        <f t="shared" ref="H3:H9" si="4">F3*COS(G3*PI()/180)</f>
-        <v>0</v>
+        <f t="shared" ref="H3:H5" si="4">F3*COS(G3*PI()/180)</f>
+        <v>-88.378860391234937</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I9" si="5">F3*SIN(G3*PI()/180)</f>
-        <v>0</v>
+        <f t="shared" ref="I3:I5" si="5">F3*SIN(G3*PI()/180)</f>
+        <v>272.00216366041394</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4017,13 +4027,19 @@
         <f t="shared" si="1"/>
         <v>24.388555609211824</v>
       </c>
+      <c r="F4">
+        <v>541</v>
+      </c>
+      <c r="G4">
+        <v>200</v>
+      </c>
       <c r="H4">
-        <f t="shared" ref="H4" si="6">F4*COS(G4*PI()/180)</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>-508.37370784517645</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4" si="7">F4*SIN(G4*PI()/180)</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>-185.03289753918673</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -4041,13 +4057,19 @@
         <f t="shared" si="1"/>
         <v>32.297247343530017</v>
       </c>
+      <c r="F5">
+        <v>390</v>
+      </c>
+      <c r="G5">
+        <v>289</v>
+      </c>
       <c r="H5">
-        <f t="shared" ref="H5" si="8">F5*COS(G5*PI()/180)</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>126.97158023829095</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5" si="9">F5*SIN(G5*PI()/180)</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>-368.75224448373359</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -4066,12 +4088,10 @@
         <v>40.178797406670412</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H9" si="10">F6*COS(G6*PI()/180)</f>
-        <v>0</v>
+        <v>46.4</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:I9" si="11">F6*SIN(G6*PI()/180)</f>
-        <v>0</v>
+        <v>52.05</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -4090,12 +4110,10 @@
         <v>47.978564639852934</v>
       </c>
       <c r="H7">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <v>-25.808872000000001</v>
       </c>
       <c r="I7">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-64.792016000000004</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -4114,11 +4132,11 @@
         <v>55.694289936152394</v>
       </c>
       <c r="H8">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="H7:H9" si="6">F8*COS(G8*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="I8">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="I7:I9" si="7">F8*SIN(G8*PI()/180)</f>
         <v>0</v>
       </c>
     </row>
@@ -4138,11 +4156,11 @@
         <v>63.323760936829771</v>
       </c>
       <c r="H9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -4410,11 +4428,11 @@
         <v>25</v>
       </c>
       <c r="C26">
-        <f t="shared" ref="C26:C89" si="12">A26*COS(B26*PI()/180)</f>
+        <f t="shared" ref="C26:C89" si="8">A26*COS(B26*PI()/180)</f>
         <v>405.1195808053825</v>
       </c>
       <c r="D26">
-        <f t="shared" ref="D26:D89" si="13">A26*SIN(B26*PI()/180)</f>
+        <f t="shared" ref="D26:D89" si="9">A26*SIN(B26*PI()/180)</f>
         <v>188.91036299809264</v>
       </c>
     </row>
@@ -4426,11 +4444,11 @@
         <v>26</v>
       </c>
       <c r="C27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>402.65973274202685</v>
       </c>
       <c r="D27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>196.39027376150668</v>
       </c>
     </row>
@@ -4442,11 +4460,11 @@
         <v>27</v>
       </c>
       <c r="C28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>400.06192936057721</v>
       </c>
       <c r="D28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>203.84173438305649</v>
       </c>
     </row>
@@ -4458,11 +4476,11 @@
         <v>28</v>
       </c>
       <c r="C29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>396.44346919365825</v>
       </c>
       <c r="D29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>210.79273169086497</v>
       </c>
     </row>
@@ -4474,11 +4492,11 @@
         <v>29</v>
       </c>
       <c r="C30">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>394.45348791986748</v>
       </c>
       <c r="D30">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>218.64913873109802</v>
       </c>
     </row>
@@ -4490,11 +4508,11 @@
         <v>30</v>
       </c>
       <c r="C31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>391.4434825105663</v>
       </c>
       <c r="D31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>225.99999999999997</v>
       </c>
     </row>
@@ -4506,11 +4524,11 @@
         <v>31</v>
       </c>
       <c r="C32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>389.15395451875901</v>
       </c>
       <c r="D32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>233.8272860091646</v>
       </c>
     </row>
@@ -4522,11 +4540,11 @@
         <v>32</v>
       </c>
       <c r="C33">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>385.86188375117382</v>
       </c>
       <c r="D33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>241.11326522610824</v>
       </c>
     </row>
@@ -4538,11 +4556,11 @@
         <v>33</v>
       </c>
       <c r="C34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>383.2724495510588</v>
       </c>
       <c r="D34">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>248.90003900186738</v>
       </c>
     </row>
@@ -4554,11 +4572,11 @@
         <v>34</v>
       </c>
       <c r="C35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>380.5282458027641</v>
       </c>
       <c r="D35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>256.66954269307286</v>
       </c>
     </row>
@@ -4570,11 +4588,11 @@
         <v>35</v>
       </c>
       <c r="C36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>377.62909241722519</v>
       </c>
       <c r="D36">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>264.41873715783225</v>
       </c>
     </row>
@@ -4586,11 +4604,11 @@
         <v>36</v>
       </c>
       <c r="C37">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>374.57486839560067</v>
       </c>
       <c r="D37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>272.14457181141506</v>
       </c>
     </row>
@@ -4602,11 +4620,11 @@
         <v>37</v>
       </c>
       <c r="C38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>371.36551217199116</v>
       </c>
       <c r="D38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>279.84398576570243</v>
       </c>
     </row>
@@ -4618,11 +4636,11 @@
         <v>38</v>
       </c>
       <c r="C39">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>368.78903268794591</v>
       </c>
       <c r="D39">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>288.12957045240802</v>
       </c>
     </row>
@@ -4634,11 +4652,11 @@
         <v>39</v>
       </c>
       <c r="C40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>366.03574784623328</v>
       </c>
       <c r="D40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>296.40990418447342</v>
       </c>
     </row>
@@ -4650,11 +4668,11 @@
         <v>40</v>
       </c>
       <c r="C41">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>363.10506603839559</v>
       </c>
       <c r="D41">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>304.68132699141961</v>
       </c>
     </row>
@@ -4666,11 +4684,11 @@
         <v>41</v>
       </c>
       <c r="C42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>359.99646976626229</v>
       </c>
       <c r="D42">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>312.94015682847191</v>
       </c>
     </row>
@@ -4682,11 +4700,11 @@
         <v>42</v>
       </c>
       <c r="C43">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>356.70951622914924</v>
       </c>
       <c r="D43">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>321.18269105225193</v>
       </c>
     </row>
@@ -4698,11 +4716,11 @@
         <v>43</v>
       </c>
       <c r="C44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>353.24383788205938</v>
       </c>
       <c r="D44">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>329.40520791018679</v>
       </c>
     </row>
@@ -4714,11 +4732,11 @@
         <v>44</v>
       </c>
       <c r="C45">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>349.59914296458447</v>
       </c>
       <c r="D45">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>337.60396804307265</v>
       </c>
     </row>
@@ -4730,11 +4748,11 @@
         <v>45</v>
       </c>
       <c r="C46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>346.4823227814083</v>
       </c>
       <c r="D46">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>346.48232278140824</v>
       </c>
     </row>
@@ -4746,11 +4764,11 @@
         <v>46</v>
       </c>
       <c r="C47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>343.16123500674468</v>
       </c>
       <c r="D47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>355.35386136729363</v>
       </c>
     </row>
@@ -4762,11 +4780,11 @@
         <v>47</v>
       </c>
       <c r="C48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>339.63518331112425</v>
       </c>
       <c r="D48">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>364.21414340634686</v>
       </c>
     </row>
@@ -4778,11 +4796,11 @@
         <v>48</v>
       </c>
       <c r="C49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>336.57269499850571</v>
       </c>
       <c r="D49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>373.80184721512927</v>
       </c>
     </row>
@@ -4794,11 +4812,11 @@
         <v>49</v>
       </c>
       <c r="C50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>332.62192769818716</v>
       </c>
       <c r="D50">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>382.63775717294538</v>
       </c>
     </row>
@@ -4810,11 +4828,11 @@
         <v>50</v>
       </c>
       <c r="C51">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>328.46446854982162</v>
       </c>
       <c r="D51">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>391.44871043379777</v>
       </c>
     </row>
@@ -4826,11 +4844,11 @@
         <v>51</v>
       </c>
       <c r="C52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>324.72932178171612</v>
       </c>
       <c r="D52">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>401.00731611179691</v>
       </c>
     </row>
@@ -4842,11 +4860,11 @@
         <v>52</v>
       </c>
       <c r="C53">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>321.37529011999362</v>
       </c>
       <c r="D53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>411.34161338270889</v>
       </c>
     </row>
@@ -4858,11 +4876,11 @@
         <v>53</v>
       </c>
       <c r="C54">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>312.34199701591314</v>
       </c>
       <c r="D54">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>414.49182971454496</v>
       </c>
     </row>
@@ -4874,11 +4892,11 @@
         <v>54</v>
       </c>
       <c r="C55">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>297.41933765999141</v>
       </c>
       <c r="D55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>409.36259915372341</v>
       </c>
     </row>
@@ -4890,11 +4908,11 @@
         <v>55</v>
       </c>
       <c r="C56">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>108.40594647034773</v>
       </c>
       <c r="D56">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>154.81973637061944</v>
       </c>
     </row>
@@ -4906,11 +4924,11 @@
         <v>56</v>
       </c>
       <c r="C57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>98.417951010851439</v>
       </c>
       <c r="D57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>145.91061276968733</v>
       </c>
     </row>
@@ -4922,11 +4940,11 @@
         <v>57</v>
       </c>
       <c r="C58">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>94.767192092614735</v>
       </c>
       <c r="D58">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>145.92867882250377</v>
       </c>
     </row>
@@ -4938,11 +4956,11 @@
         <v>58</v>
       </c>
       <c r="C59">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>91.676032712344451</v>
       </c>
       <c r="D59">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>146.7123206350617</v>
       </c>
     </row>
@@ -4954,11 +4972,11 @@
         <v>59</v>
       </c>
       <c r="C60">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>88.58654888452935</v>
       </c>
       <c r="D60">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>147.43277572076329</v>
       </c>
     </row>
@@ -4970,11 +4988,11 @@
         <v>60</v>
       </c>
       <c r="C61">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>85.000000000000014</v>
       </c>
       <c r="D61">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>147.22431864335456</v>
       </c>
     </row>
@@ -4986,11 +5004,11 @@
         <v>61</v>
       </c>
       <c r="C62">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>81.932825821630971</v>
       </c>
       <c r="D62">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>147.81073050655789</v>
       </c>
     </row>
@@ -5002,11 +5020,11 @@
         <v>62</v>
       </c>
       <c r="C63">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>78.871222548029664</v>
       </c>
       <c r="D63">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>148.33519560029973</v>
       </c>
     </row>
@@ -5018,11 +5036,11 @@
         <v>63</v>
       </c>
       <c r="C64">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>75.816413456504321</v>
       </c>
       <c r="D64">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>148.79808953945741</v>
       </c>
     </row>
@@ -5034,11 +5052,11 @@
         <v>64</v>
       </c>
       <c r="C65">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>72.769610366986853</v>
       </c>
       <c r="D65">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>149.19981168566173</v>
       </c>
     </row>
@@ -5050,11 +5068,11 @@
         <v>65</v>
       </c>
       <c r="C66">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>70.15463144895611</v>
       </c>
       <c r="D66">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>150.4470926480839</v>
       </c>
     </row>
@@ -5066,11 +5084,11 @@
         <v>66</v>
       </c>
       <c r="C67">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>67.92501939365863</v>
       </c>
       <c r="D67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>152.56209142631434</v>
       </c>
     </row>
@@ -5082,11 +5100,11 @@
         <v>67</v>
       </c>
       <c r="C68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>65.642829586198019</v>
       </c>
       <c r="D68">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>154.64481538000996</v>
       </c>
     </row>
@@ -5098,11 +5116,11 @@
         <v>68</v>
       </c>
       <c r="C69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>64.057727474120952</v>
       </c>
       <c r="D69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>158.54843913092066</v>
       </c>
     </row>
@@ -5114,11 +5132,11 @@
         <v>69</v>
       </c>
       <c r="C70">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>61.997655271336967</v>
       </c>
       <c r="D70">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>161.50941378401589</v>
       </c>
     </row>
@@ -5130,11 +5148,11 @@
         <v>70</v>
       </c>
       <c r="C71">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>60.537565368643385</v>
       </c>
       <c r="D71">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>166.32559387910578</v>
       </c>
     </row>
@@ -5146,11 +5164,11 @@
         <v>71</v>
       </c>
       <c r="C72">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>59.253404111202528</v>
       </c>
       <c r="D72">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>172.08438075907566</v>
       </c>
     </row>
@@ -5162,11 +5180,11 @@
         <v>72</v>
       </c>
       <c r="C73">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>-0.30901699437494745</v>
       </c>
       <c r="D73">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>-0.95105651629515353</v>
       </c>
     </row>
@@ -5178,11 +5196,11 @@
         <v>73</v>
       </c>
       <c r="C74">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>-0.29237170472273677</v>
       </c>
       <c r="D74">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>-0.95630475596303544</v>
       </c>
     </row>
@@ -5194,11 +5212,11 @@
         <v>74</v>
       </c>
       <c r="C75">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>-0.27563735581699916</v>
       </c>
       <c r="D75">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>-0.96126169593831889</v>
       </c>
     </row>
@@ -5210,11 +5228,11 @@
         <v>75</v>
       </c>
       <c r="C76">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>-0.25881904510252074</v>
       </c>
       <c r="D76">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>-0.96592582628906831</v>
       </c>
     </row>
@@ -5226,11 +5244,11 @@
         <v>76</v>
       </c>
       <c r="C77">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>-0.2419218955996679</v>
       </c>
       <c r="D77">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>-0.97029572627599647</v>
       </c>
     </row>
@@ -5242,11 +5260,11 @@
         <v>77</v>
       </c>
       <c r="C78">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>75.583554259538616</v>
       </c>
       <c r="D78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>327.38834176783905</v>
       </c>
     </row>
@@ -5258,11 +5276,11 @@
         <v>78</v>
       </c>
       <c r="C79">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>69.026681351496137</v>
       </c>
       <c r="D79">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>324.74500344362343</v>
       </c>
     </row>
@@ -5274,11 +5292,11 @@
         <v>79</v>
       </c>
       <c r="C80">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>62.77615947888328</v>
       </c>
       <c r="D80">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>322.95534335428147</v>
       </c>
     </row>
@@ -5290,11 +5308,11 @@
         <v>80</v>
       </c>
       <c r="C81">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>56.609305919419313</v>
       </c>
       <c r="D81">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>321.04732748197983</v>
       </c>
     </row>
@@ -5306,11 +5324,11 @@
         <v>81</v>
       </c>
       <c r="C82">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>50.528332207994588</v>
       </c>
       <c r="D82">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>319.0233340122295</v>
       </c>
     </row>
@@ -5322,11 +5340,11 @@
         <v>82</v>
       </c>
       <c r="C83">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>44.535392307221016</v>
       </c>
       <c r="D83">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>316.8857819973025</v>
       </c>
     </row>
@@ -5338,11 +5356,11 @@
         <v>83</v>
       </c>
       <c r="C84">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>38.632581859431752</v>
       </c>
       <c r="D84">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>314.63713007029907</v>
       </c>
     </row>
@@ -5354,11 +5372,11 @@
         <v>84</v>
       </c>
       <c r="C85">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>32.821937466043188</v>
       </c>
       <c r="D85">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>312.27987514563779</v>
       </c>
     </row>
@@ -5370,11 +5388,11 @@
         <v>85</v>
       </c>
       <c r="C86">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>27.192591737269339</v>
       </c>
       <c r="D86">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>310.81274580462463</v>
       </c>
     </row>
@@ -5386,11 +5404,11 @@
         <v>86</v>
       </c>
       <c r="C87">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>21.554750386934767</v>
       </c>
       <c r="D87">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>308.24729153028568</v>
       </c>
     </row>
@@ -5402,11 +5420,11 @@
         <v>87</v>
       </c>
       <c r="C88">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>16.067138566583797</v>
       </c>
       <c r="D88">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>306.57926716965414</v>
       </c>
     </row>
@@ -5418,11 +5436,11 @@
         <v>88</v>
       </c>
       <c r="C89">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>10.64434649426283</v>
       </c>
       <c r="D89">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>304.81420224082422</v>
       </c>
     </row>
@@ -5434,11 +5452,11 @@
         <v>89</v>
       </c>
       <c r="C90">
-        <f t="shared" ref="C90:C153" si="14">A90*COS(B90*PI()/180)</f>
+        <f t="shared" ref="C90:C153" si="10">A90*COS(B90*PI()/180)</f>
         <v>5.3055315569341461</v>
       </c>
       <c r="D90">
-        <f t="shared" ref="D90:D153" si="15">A90*SIN(B90*PI()/180)</f>
+        <f t="shared" ref="D90:D153" si="11">A90*SIN(B90*PI()/180)</f>
         <v>303.95369932754295</v>
       </c>
     </row>
@@ -5450,11 +5468,11 @@
         <v>90</v>
       </c>
       <c r="C91">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>1.8438484246374731E-14</v>
       </c>
       <c r="D91">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>301</v>
       </c>
     </row>
@@ -5466,11 +5484,11 @@
         <v>91</v>
       </c>
       <c r="C92">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-5.2357219311850427</v>
       </c>
       <c r="D92">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>299.95430854691739</v>
       </c>
     </row>
@@ -5482,11 +5500,11 @@
         <v>92</v>
       </c>
       <c r="C93">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-10.400050017345219</v>
       </c>
       <c r="D93">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>297.81846645169054</v>
       </c>
     </row>
@@ -5498,11 +5516,11 @@
         <v>93</v>
       </c>
       <c r="C94">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-15.491443047911311</v>
       </c>
       <c r="D94">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>295.59434228735387</v>
       </c>
     </row>
@@ -5514,11 +5532,11 @@
         <v>94</v>
       </c>
       <c r="C95">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-20.578159754516971</v>
       </c>
       <c r="D95">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>294.28139482664812</v>
       </c>
     </row>
@@ -5530,11 +5548,11 @@
         <v>95</v>
       </c>
       <c r="C96">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-25.623788367811521</v>
       </c>
       <c r="D96">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>292.88124123897319</v>
       </c>
     </row>
@@ -5546,11 +5564,11 @@
         <v>96</v>
       </c>
       <c r="C97">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-30.626839737422426</v>
       </c>
       <c r="D97">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>291.39491534290408</v>
       </c>
     </row>
@@ -5562,11 +5580,11 @@
         <v>97</v>
       </c>
       <c r="C98">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-35.585848274303032</v>
       </c>
       <c r="D98">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>289.82347627926606</v>
       </c>
     </row>
@@ -5578,11 +5596,11 @@
         <v>98</v>
       </c>
       <c r="C99">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-40.499372379379018</v>
       </c>
       <c r="D99">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>288.16800800379696</v>
       </c>
     </row>
@@ -5594,11 +5612,11 @@
         <v>99</v>
       </c>
       <c r="C100">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-45.365994861666998</v>
       </c>
       <c r="D100">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>286.42961877258995</v>
       </c>
     </row>
@@ -5610,11 +5628,11 @@
         <v>100</v>
       </c>
       <c r="C101">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-50.184323345742861</v>
       </c>
       <c r="D101">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>284.60944062052812</v>
       </c>
     </row>
@@ -5626,11 +5644,11 @@
         <v>101</v>
       </c>
       <c r="C102">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-55.143799663821447</v>
       </c>
       <c r="D102">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>283.69025601637492</v>
       </c>
     </row>
@@ -5642,11 +5660,11 @@
         <v>102</v>
       </c>
       <c r="C103">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-59.878566955514628</v>
       </c>
       <c r="D103">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>281.70650901133604</v>
       </c>
     </row>
@@ -5658,11 +5676,11 @@
         <v>103</v>
       </c>
       <c r="C104">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-64.560952596689205</v>
       </c>
       <c r="D104">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>279.64420859336252</v>
       </c>
     </row>
@@ -5674,11 +5692,11 @@
         <v>104</v>
       </c>
       <c r="C105">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-69.431584037104656</v>
       </c>
       <c r="D105">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>278.474873441211</v>
       </c>
     </row>
@@ -5690,11 +5708,11 @@
         <v>105</v>
       </c>
       <c r="C106">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-74.281065944423489</v>
       </c>
       <c r="D106">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>277.22071214496259</v>
       </c>
     </row>
@@ -5706,11 +5724,11 @@
         <v>106</v>
       </c>
       <c r="C107">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-79.107921119478732</v>
       </c>
       <c r="D107">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>275.88210673429751</v>
       </c>
     </row>
@@ -5722,11 +5740,11 @@
         <v>107</v>
       </c>
       <c r="C108">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-83.910679255425421</v>
       </c>
       <c r="D108">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>274.45946496139118</v>
       </c>
     </row>
@@ -5738,11 +5756,11 @@
         <v>108</v>
       </c>
       <c r="C109">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-88.68787738560988</v>
       </c>
       <c r="D109">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>272.95322017670912</v>
       </c>
     </row>
@@ -5754,11 +5772,11 @@
         <v>109</v>
       </c>
       <c r="C110">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-93.438060329203893</v>
       </c>
       <c r="D110">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>271.36383119700395</v>
       </c>
     </row>
@@ -5770,11 +5788,11 @@
         <v>110</v>
       </c>
       <c r="C111">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-98.159781134466925</v>
       </c>
       <c r="D111">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>269.69178216555571</v>
       </c>
     </row>
@@ -5786,11 +5804,11 @@
         <v>111</v>
       </c>
       <c r="C112">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-102.85160151950117</v>
       </c>
       <c r="D112">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>267.93758240469691</v>
       </c>
     </row>
@@ -5802,11 +5820,11 @@
         <v>112</v>
       </c>
       <c r="C113">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-107.51209231036677</v>
       </c>
       <c r="D113">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>266.101766260668</v>
       </c>
     </row>
@@ -5818,11 +5836,11 @@
         <v>113</v>
       </c>
       <c r="C114">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-112.5305650049108</v>
       </c>
       <c r="D114">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>265.1053977943028</v>
       </c>
     </row>
@@ -5834,11 +5852,11 @@
         <v>114</v>
       </c>
       <c r="C115">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-117.14015320583042</v>
       </c>
       <c r="D115">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>263.10109180106906</v>
       </c>
     </row>
@@ -5850,11 +5868,11 @@
         <v>115</v>
       </c>
       <c r="C116">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-121.71405938132141</v>
       </c>
       <c r="D116">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>261.01664266655519</v>
       </c>
     </row>
@@ -5866,11 +5884,11 @@
         <v>116</v>
       </c>
       <c r="C117">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-126.6892614220434</v>
       </c>
       <c r="D117">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>259.75147938045922</v>
       </c>
     </row>
@@ -5882,11 +5900,11 @@
         <v>117</v>
       </c>
       <c r="C118">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-131.65724492446853</v>
       </c>
       <c r="D118">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>258.39189201462671</v>
       </c>
     </row>
@@ -5898,11 +5916,11 @@
         <v>118</v>
       </c>
       <c r="C119">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-136.61622477069415</v>
       </c>
       <c r="D119">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>256.93774952194781</v>
       </c>
     </row>
@@ -5914,11 +5932,11 @@
         <v>119</v>
       </c>
       <c r="C120">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-141.56440911193042</v>
       </c>
       <c r="D120">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>255.38895448470359</v>
       </c>
     </row>
@@ -5930,11 +5948,11 @@
         <v>120</v>
       </c>
       <c r="C121">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-146.99999999999994</v>
       </c>
       <c r="D121">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>254.61146871262497</v>
       </c>
     </row>
@@ -5946,11 +5964,11 @@
         <v>121</v>
       </c>
       <c r="C122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-151.93623209846601</v>
       </c>
       <c r="D122">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>252.86435370712314</v>
       </c>
     </row>
@@ -5962,11 +5980,11 @@
         <v>122</v>
       </c>
       <c r="C123">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-157.38602147726183</v>
       </c>
       <c r="D123">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>251.87028455845854</v>
       </c>
     </row>
@@ -5978,11 +5996,11 @@
         <v>123</v>
       </c>
       <c r="C124">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-162.8470714694931</v>
       </c>
       <c r="D124">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>250.76249981568176</v>
       </c>
     </row>
@@ -5994,11 +6012,11 @@
         <v>124</v>
       </c>
       <c r="C125">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-168.31706394469475</v>
       </c>
       <c r="D125">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>249.54030933906756</v>
       </c>
     </row>
@@ -6010,11 +6028,11 @@
         <v>125</v>
       </c>
       <c r="C126">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-173.79366021436689</v>
       </c>
       <c r="D126">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>248.20306941956457</v>
       </c>
     </row>
@@ -6026,11 +6044,11 @@
         <v>126</v>
       </c>
       <c r="C127">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-179.86228720149674</v>
       </c>
       <c r="D127">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>247.55920027873393</v>
       </c>
     </row>
@@ -6042,11 +6060,11 @@
         <v>127</v>
       </c>
       <c r="C128">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-185.3590271308309</v>
       </c>
       <c r="D128">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>245.97973709456616</v>
       </c>
     </row>
@@ -6058,11 +6076,11 @@
         <v>128</v>
       </c>
       <c r="C129">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-190.85505735095407</v>
       </c>
       <c r="D129">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>244.28333361808382</v>
       </c>
     </row>
@@ -6074,11 +6092,11 @@
         <v>129</v>
       </c>
       <c r="C130">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-196.97728239859907</v>
       </c>
       <c r="D130">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>243.24668593603192</v>
       </c>
     </row>
@@ -6090,11 +6108,11 @@
         <v>130</v>
       </c>
       <c r="C131">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-202.47809705125991</v>
       </c>
       <c r="D131">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>241.30399958247807</v>
       </c>
     </row>
@@ -6106,11 +6124,11 @@
         <v>131</v>
       </c>
       <c r="C132">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-209.2828302479719</v>
       </c>
       <c r="D132">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>240.7523560910642</v>
       </c>
     </row>
@@ -6122,11 +6140,11 @@
         <v>132</v>
       </c>
       <c r="C133">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-214.7909246411935</v>
       </c>
       <c r="D133">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>238.54948897824355</v>
       </c>
     </row>
@@ -6138,11 +6156,11 @@
         <v>133</v>
       </c>
       <c r="C134">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-221.64946702031196</v>
       </c>
       <c r="D134">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>237.68995302623043</v>
       </c>
     </row>
@@ -6154,11 +6172,11 @@
         <v>134</v>
       </c>
       <c r="C135">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-227.84794551055103</v>
       </c>
       <c r="D135">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>235.94345451107768</v>
       </c>
     </row>
@@ -6170,11 +6188,11 @@
         <v>135</v>
       </c>
       <c r="C136">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-234.05234457274722</v>
       </c>
       <c r="D136">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>234.05234457274724</v>
       </c>
     </row>
@@ -6186,11 +6204,11 @@
         <v>136</v>
       </c>
       <c r="C137">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-240.25949331310949</v>
       </c>
       <c r="D137">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>232.01589573330506</v>
       </c>
     </row>
@@ -6202,11 +6220,11 @@
         <v>137</v>
       </c>
       <c r="C138">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-247.19755114727963</v>
       </c>
       <c r="D138">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>230.51544570112452</v>
       </c>
     </row>
@@ -6218,11 +6236,11 @@
         <v>138</v>
       </c>
       <c r="C139">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-254.15553031326874</v>
       </c>
       <c r="D139">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>228.84266737472956</v>
       </c>
     </row>
@@ -6234,11 +6252,11 @@
         <v>139</v>
       </c>
       <c r="C140">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-261.88422433730187</v>
       </c>
       <c r="D140">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>227.65248305970601</v>
       </c>
     </row>
@@ -6250,11 +6268,11 @@
         <v>140</v>
       </c>
       <c r="C141">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-268.11555509164225</v>
       </c>
       <c r="D141">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>224.97566339028882</v>
       </c>
     </row>
@@ -6266,11 +6284,11 @@
         <v>141</v>
       </c>
       <c r="C142">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-275.8868163172246</v>
       </c>
       <c r="D142">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>223.40873882269238</v>
       </c>
     </row>
@@ -6282,11 +6300,11 @@
         <v>142</v>
       </c>
       <c r="C143">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-283.68387129841989</v>
       </c>
       <c r="D143">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>221.63813111723704</v>
       </c>
     </row>
@@ -6298,11 +6316,11 @@
         <v>143</v>
       </c>
       <c r="C144">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-291.50196116726192</v>
       </c>
       <c r="D144">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>219.66248345049758</v>
       </c>
     </row>
@@ -6314,11 +6332,11 @@
         <v>144</v>
       </c>
       <c r="C145">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-299.33628791873053</v>
       </c>
       <c r="D145">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>217.48054334821509</v>
       </c>
     </row>
@@ -6330,11 +6348,11 @@
         <v>145</v>
       </c>
       <c r="C146">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-308.00116865266085</v>
       </c>
       <c r="D146">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>215.66474006799345</v>
       </c>
     </row>
@@ -6346,11 +6364,11 @@
         <v>146</v>
       </c>
       <c r="C147">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-315.86331514347086</v>
       </c>
       <c r="D147">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>213.05249622235456</v>
       </c>
     </row>
@@ -6362,11 +6380,11 @@
         <v>147</v>
       </c>
       <c r="C148">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-324.56550979487918</v>
       </c>
       <c r="D148">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>210.77530655081543</v>
       </c>
     </row>
@@ -6378,11 +6396,11 @@
         <v>148</v>
       </c>
       <c r="C149">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-333.28290178947537</v>
       </c>
       <c r="D149">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>208.25827084364951</v>
       </c>
     </row>
@@ -6394,11 +6412,11 @@
         <v>149</v>
       </c>
       <c r="C150">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-342.00975298014276</v>
       </c>
       <c r="D150">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>205.5001918891117</v>
       </c>
     </row>
@@ -6410,11 +6428,11 @@
         <v>150</v>
       </c>
       <c r="C151">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-351.60631393648214</v>
       </c>
       <c r="D151">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>202.99999999999997</v>
       </c>
     </row>
@@ -6426,11 +6444,11 @@
         <v>151</v>
       </c>
       <c r="C152">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-361.21793904857043</v>
       </c>
       <c r="D152">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>200.22637316173726</v>
       </c>
     </row>
@@ -6442,11 +6460,11 @@
         <v>152</v>
       </c>
       <c r="C153">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>-370.83798900074925</v>
       </c>
       <c r="D153">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>197.17805637007424</v>
       </c>
     </row>
@@ -6458,11 +6476,11 @@
         <v>153</v>
       </c>
       <c r="C154">
-        <f t="shared" ref="C154:C217" si="16">A154*COS(B154*PI()/180)</f>
+        <f t="shared" ref="C154:C217" si="12">A154*COS(B154*PI()/180)</f>
         <v>-381.3507923526214</v>
       </c>
       <c r="D154">
-        <f t="shared" ref="D154:D217" si="17">A154*SIN(B154*PI()/180)</f>
+        <f t="shared" ref="D154:D217" si="13">A154*SIN(B154*PI()/180)</f>
         <v>194.30793388852607</v>
       </c>
     </row>
@@ -6474,11 +6492,11 @@
         <v>154</v>
       </c>
       <c r="C155">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-390.07661609383848</v>
       </c>
       <c r="D155">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>190.25307770645955</v>
       </c>
     </row>
@@ -6490,11 +6508,11 @@
         <v>155</v>
       </c>
       <c r="C156">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-399.68173408316261</v>
       </c>
       <c r="D156">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>186.37465342764847</v>
       </c>
     </row>
@@ -6506,11 +6524,11 @@
         <v>156</v>
       </c>
       <c r="C157">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-409.26836502388517</v>
       </c>
       <c r="D157">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>182.21801609795858</v>
       </c>
     </row>
@@ -6522,11 +6540,11 @@
         <v>157</v>
       </c>
       <c r="C158">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-418.82970832086028</v>
       </c>
       <c r="D158">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>177.78266346261975</v>
       </c>
     </row>
@@ -6538,11 +6556,11 @@
         <v>158</v>
       </c>
       <c r="C159">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-429.28612466442252</v>
       </c>
       <c r="D159">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>173.44285275156736</v>
       </c>
     </row>
@@ -6554,11 +6572,11 @@
         <v>159</v>
       </c>
       <c r="C160">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-439.71638088018204</v>
       </c>
       <c r="D160">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>168.79130423583641</v>
       </c>
     </row>
@@ -6570,11 +6588,11 @@
         <v>160</v>
       </c>
       <c r="C161">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-451.05245797723597</v>
       </c>
       <c r="D161">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>164.16966879632105</v>
       </c>
     </row>
@@ -6586,11 +6604,11 @@
         <v>161</v>
       </c>
       <c r="C162">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-462.35858346806589</v>
       </c>
       <c r="D162">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>159.20282752954978</v>
       </c>
     </row>
@@ -6602,11 +6620,11 @@
         <v>162</v>
       </c>
       <c r="C163">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-474.57720163128164</v>
       </c>
       <c r="D163">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>154.19948019309879</v>
       </c>
     </row>
@@ -6618,11 +6636,11 @@
         <v>163</v>
       </c>
       <c r="C164">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-486.75912078518502</v>
       </c>
       <c r="D164">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>148.81719770387315</v>
       </c>
     </row>
@@ -6634,11 +6652,11 @@
         <v>164</v>
       </c>
       <c r="C165">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-498.89482019198738</v>
       </c>
       <c r="D165">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>143.05578766902283</v>
       </c>
     </row>
@@ -6650,11 +6668,11 @@
         <v>165</v>
       </c>
       <c r="C166">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-176.76442621089947</v>
       </c>
       <c r="D166">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>47.363885253761346</v>
       </c>
     </row>
@@ -6666,11 +6684,11 @@
         <v>166</v>
       </c>
       <c r="C167">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-161.06909056181541</v>
       </c>
       <c r="D167">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>40.159034669544845</v>
       </c>
     </row>
@@ -6682,11 +6700,11 @@
         <v>167</v>
       </c>
       <c r="C168">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-154.9248403008524</v>
       </c>
       <c r="D168">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>35.767217640674502</v>
       </c>
     </row>
@@ -6698,11 +6716,11 @@
         <v>168</v>
       </c>
       <c r="C169">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-152.59102571447369</v>
       </c>
       <c r="D169">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>32.434223767570451</v>
       </c>
     </row>
@@ -6714,11 +6732,11 @@
         <v>169</v>
       </c>
       <c r="C170">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-151.17058625094026</v>
       </c>
       <c r="D170">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>29.384585287987925</v>
       </c>
     </row>
@@ -6730,11 +6748,11 @@
         <v>170</v>
       </c>
       <c r="C171">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-149.69077845785563</v>
       </c>
       <c r="D171">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>26.394523005373401</v>
       </c>
     </row>
@@ -6746,11 +6764,11 @@
         <v>171</v>
       </c>
       <c r="C172">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-148.15325108927064</v>
       </c>
       <c r="D172">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>23.465169756034648</v>
       </c>
     </row>
@@ -6762,11 +6780,11 @@
         <v>172</v>
       </c>
       <c r="C173">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-147.54994224249396</v>
       </c>
       <c r="D173">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>20.736792043049796</v>
       </c>
     </row>
@@ -6778,11 +6796,11 @@
         <v>173</v>
       </c>
       <c r="C174">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-147.88937659455698</v>
       </c>
       <c r="D174">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>18.158532167366985</v>
       </c>
     </row>
@@ -6794,11 +6812,11 @@
         <v>174</v>
       </c>
       <c r="C175">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-147.18924051450443</v>
       </c>
       <c r="D175">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>15.470212563612753</v>
       </c>
     </row>
@@ -6810,11 +6828,11 @@
         <v>175</v>
       </c>
       <c r="C176">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-147.43681531757835</v>
       </c>
       <c r="D176">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>12.899049926653479</v>
       </c>
     </row>
@@ -6826,11 +6844,11 @@
         <v>176</v>
       </c>
       <c r="C177">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-147.63947943845398</v>
       </c>
       <c r="D177">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>10.323958114130578</v>
       </c>
     </row>
@@ -6842,11 +6860,11 @@
         <v>177</v>
       </c>
       <c r="C178">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-148.7958006784315</v>
       </c>
       <c r="D178">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>7.7980574801986275</v>
       </c>
     </row>
@@ -6858,11 +6876,11 @@
         <v>178</v>
       </c>
       <c r="C179">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-149.90862405286435</v>
       </c>
       <c r="D179">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>5.2349245053751048</v>
       </c>
     </row>
@@ -6874,11 +6892,11 @@
         <v>179</v>
       </c>
       <c r="C180">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-151.97684966377147</v>
       </c>
       <c r="D180">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>2.6527657784670828</v>
       </c>
     </row>
@@ -6890,11 +6908,11 @@
         <v>180</v>
       </c>
       <c r="C181">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-153</v>
       </c>
       <c r="D181">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>1.8744771360101886E-14</v>
       </c>
     </row>
@@ -6906,11 +6924,11 @@
         <v>181</v>
       </c>
       <c r="C182">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-153.97654505408426</v>
       </c>
       <c r="D182">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-2.6876705913416115</v>
       </c>
     </row>
@@ -6922,11 +6940,11 @@
         <v>182</v>
       </c>
       <c r="C183">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-155.90496901497895</v>
       </c>
       <c r="D183">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-5.4443214855901401</v>
       </c>
     </row>
@@ -6938,11 +6956,11 @@
         <v>183</v>
       </c>
       <c r="C184">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-159.78072556073181</v>
       </c>
       <c r="D184">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-8.3737529988709696</v>
       </c>
     </row>
@@ -6954,11 +6972,11 @@
         <v>184</v>
       </c>
       <c r="C185">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-162.60294019235135</v>
       </c>
       <c r="D185">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-11.370305220292348</v>
       </c>
     </row>
@@ -6970,11 +6988,11 @@
         <v>185</v>
       </c>
       <c r="C186">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>0.99619469809174555</v>
       </c>
       <c r="D186">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>8.7155742747657944E-2</v>
       </c>
     </row>
@@ -6986,11 +7004,11 @@
         <v>186</v>
       </c>
       <c r="C187">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>0.9945218953682734</v>
       </c>
       <c r="D187">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>0.10452846326765305</v>
       </c>
     </row>
@@ -7002,11 +7020,11 @@
         <v>187</v>
       </c>
       <c r="C188">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>0.99254615164132198</v>
       </c>
       <c r="D188">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>0.12186934340514774</v>
       </c>
     </row>
@@ -7018,11 +7036,11 @@
         <v>188</v>
       </c>
       <c r="C189">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-220.82977932937015</v>
       </c>
       <c r="D189">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-31.035601514094612</v>
       </c>
     </row>
@@ -7034,11 +7052,11 @@
         <v>189</v>
       </c>
       <c r="C190">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-223.21756497450113</v>
       </c>
       <c r="D190">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-35.354189099092146</v>
       </c>
     </row>
@@ -7050,11 +7068,11 @@
         <v>190</v>
       </c>
       <c r="C191">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-224.53616768678341</v>
       </c>
       <c r="D191">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-39.591784508060144</v>
       </c>
     </row>
@@ -7066,11 +7084,11 @@
         <v>191</v>
       </c>
       <c r="C192">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-226.75587937641038</v>
       </c>
       <c r="D192">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-44.076877931981834</v>
       </c>
     </row>
@@ -7082,11 +7100,11 @@
         <v>192</v>
       </c>
       <c r="C193">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>0.97814760073380569</v>
       </c>
       <c r="D193">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>0.20791169081775907</v>
       </c>
     </row>
@@ -7098,11 +7116,11 @@
         <v>193</v>
       </c>
       <c r="C194">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>0.97437006478523525</v>
       </c>
       <c r="D194">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>0.22495105434386498</v>
       </c>
     </row>
@@ -7114,11 +7132,11 @@
         <v>194</v>
       </c>
       <c r="C195">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-240.63334011644713</v>
       </c>
       <c r="D195">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-59.99663010871754</v>
       </c>
     </row>
@@ -7130,11 +7148,11 @@
         <v>195</v>
       </c>
       <c r="C196">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>0.96592582628906842</v>
       </c>
       <c r="D196">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>0.25881904510252035</v>
       </c>
     </row>
@@ -7146,11 +7164,11 @@
         <v>196</v>
       </c>
       <c r="C197">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-281.64967690992745</v>
       </c>
       <c r="D197">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-80.761745254380699</v>
       </c>
     </row>
@@ -7162,11 +7180,11 @@
         <v>197</v>
       </c>
       <c r="C198">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>0.95630475596303555</v>
       </c>
       <c r="D198">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>0.29237170472273638</v>
       </c>
     </row>
@@ -7178,11 +7196,11 @@
         <v>198</v>
       </c>
       <c r="C199">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>0.95105651629515353</v>
       </c>
       <c r="D199">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>0.30901699437494773</v>
       </c>
     </row>
@@ -7194,11 +7212,11 @@
         <v>199</v>
       </c>
       <c r="C200">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>0.94551857559931674</v>
       </c>
       <c r="D200">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>0.32556815445715676</v>
       </c>
     </row>
@@ -7210,11 +7228,11 @@
         <v>200</v>
       </c>
       <c r="C201">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-509.31340046596239</v>
       </c>
       <c r="D201">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-185.3749176825124</v>
       </c>
     </row>
@@ -7226,11 +7244,11 @@
         <v>201</v>
       </c>
       <c r="C202">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-506.00059116148333</v>
       </c>
       <c r="D202">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-194.23542865355284</v>
       </c>
     </row>
@@ -7242,11 +7260,11 @@
         <v>202</v>
       </c>
       <c r="C203">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-502.53364917519878</v>
       </c>
       <c r="D203">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-203.03677363142432</v>
       </c>
     </row>
@@ -7258,11 +7276,11 @@
         <v>203</v>
       </c>
       <c r="C204">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-498.91363057122271</v>
       </c>
       <c r="D204">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-211.77627164118627</v>
       </c>
     </row>
@@ -7274,11 +7292,11 @@
         <v>204</v>
       </c>
       <c r="C205">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-496.05518349993241</v>
       </c>
       <c r="D205">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-220.8579971901593</v>
       </c>
     </row>
@@ -7290,11 +7308,11 @@
         <v>205</v>
       </c>
       <c r="C206">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-493.0314361479376</v>
       </c>
       <c r="D206">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-229.90433438694041</v>
       </c>
     </row>
@@ -7306,11 +7324,11 @@
         <v>206</v>
       </c>
       <c r="C207">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-488.94396118674695</v>
       </c>
       <c r="D207">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-238.47390385325792</v>
       </c>
     </row>
@@ -7322,11 +7340,11 @@
         <v>207</v>
       </c>
       <c r="C208">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-486.48956220684897</v>
       </c>
       <c r="D208">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-247.87881285779224</v>
       </c>
     </row>
@@ -7338,11 +7356,11 @@
         <v>208</v>
       </c>
       <c r="C209">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-482.972333293833</v>
       </c>
       <c r="D209">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-256.80094484388229</v>
       </c>
     </row>
@@ -7354,11 +7372,11 @@
         <v>209</v>
       </c>
       <c r="C210">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-479.29159951238893</v>
       </c>
       <c r="D210">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-265.67567189499266</v>
       </c>
     </row>
@@ -7370,11 +7388,11 @@
         <v>210</v>
       </c>
       <c r="C211">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-475.44794667765677</v>
       </c>
       <c r="D211">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-274.50000000000006</v>
       </c>
     </row>
@@ -7386,11 +7404,11 @@
         <v>211</v>
       </c>
       <c r="C212">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-472.2991826868639</v>
       </c>
       <c r="D212">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-283.78597927543984</v>
       </c>
     </row>
@@ -7402,11 +7420,11 @@
         <v>212</v>
       </c>
       <c r="C213">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-468.97059717450361</v>
       </c>
       <c r="D213">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-293.04535312096226</v>
       </c>
     </row>
@@ -7418,11 +7436,11 @@
         <v>213</v>
       </c>
       <c r="C214">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-465.46216520971035</v>
       </c>
       <c r="D214">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-302.27466443334004</v>
       </c>
     </row>
@@ -7434,11 +7452,11 @@
         <v>214</v>
       </c>
       <c r="C215">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-462.60296548571336</v>
       </c>
       <c r="D215">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-312.02964013667668</v>
       </c>
     </row>
@@ -7450,11 +7468,11 @@
         <v>215</v>
       </c>
       <c r="C216">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-458.72514480183554</v>
       </c>
       <c r="D216">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-321.20280435658566</v>
       </c>
     </row>
@@ -7466,11 +7484,11 @@
         <v>216</v>
       </c>
       <c r="C217">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>-455.47656783309549</v>
       </c>
       <c r="D217">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>-330.9230970406623</v>
       </c>
     </row>
@@ -7482,11 +7500,11 @@
         <v>217</v>
       </c>
       <c r="C218">
-        <f t="shared" ref="C218:C281" si="18">A218*COS(B218*PI()/180)</f>
+        <f t="shared" ref="C218:C281" si="14">A218*COS(B218*PI()/180)</f>
         <v>-451.22906317672056</v>
       </c>
       <c r="D218">
-        <f t="shared" ref="D218:D281" si="19">A218*SIN(B218*PI()/180)</f>
+        <f t="shared" ref="D218:D281" si="15">A218*SIN(B218*PI()/180)</f>
         <v>-340.02548808090717</v>
       </c>
     </row>
@@ -7498,11 +7516,11 @@
         <v>218</v>
       </c>
       <c r="C219">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-289.98795732727376</v>
       </c>
       <c r="D219">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-226.56342291984208</v>
       </c>
     </row>
@@ -7514,11 +7532,11 @@
         <v>219</v>
       </c>
       <c r="C220">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-280.54969208596646</v>
       </c>
       <c r="D220">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-227.18466116899137</v>
       </c>
     </row>
@@ -7530,11 +7548,11 @@
         <v>220</v>
       </c>
       <c r="C221">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-271.17973286411819</v>
       </c>
       <c r="D221">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-227.5468138290349</v>
       </c>
     </row>
@@ -7546,11 +7564,11 @@
         <v>221</v>
       </c>
       <c r="C222">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-263.39364349774741</v>
       </c>
       <c r="D222">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-228.96460111768707</v>
       </c>
     </row>
@@ -7562,11 +7580,11 @@
         <v>222</v>
       </c>
       <c r="C223">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-251.92609583683665</v>
       </c>
       <c r="D223">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-226.83527555565294</v>
       </c>
     </row>
@@ -7578,11 +7596,11 @@
         <v>223</v>
       </c>
       <c r="C224">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-242.80942893756463</v>
       </c>
       <c r="D224">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-226.42345554074944</v>
       </c>
     </row>
@@ -7594,11 +7612,11 @@
         <v>224</v>
       </c>
       <c r="C225">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-228.03071670735238</v>
       </c>
       <c r="D225">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-220.20670343550216</v>
       </c>
     </row>
@@ -7610,11 +7628,11 @@
         <v>225</v>
       </c>
       <c r="C226">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>0.70710678118654768</v>
       </c>
       <c r="D226">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>0.70710678118654746</v>
       </c>
     </row>
@@ -7626,11 +7644,11 @@
         <v>226</v>
       </c>
       <c r="C227">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>0.69465837045899759</v>
       </c>
       <c r="D227">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>0.71933980033865086</v>
       </c>
     </row>
@@ -7642,11 +7660,11 @@
         <v>227</v>
       </c>
       <c r="C228">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-200.50751785837468</v>
       </c>
       <c r="D228">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-215.01798827603602</v>
       </c>
     </row>
@@ -7658,11 +7676,11 @@
         <v>228</v>
       </c>
       <c r="C229">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-195.38613705678668</v>
       </c>
       <c r="D229">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-216.99828903939905</v>
       </c>
     </row>
@@ -7674,11 +7692,11 @@
         <v>229</v>
       </c>
       <c r="C230">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-190.25711840724722</v>
       </c>
       <c r="D230">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-218.86577826460379</v>
       </c>
     </row>
@@ -7690,11 +7708,11 @@
         <v>230</v>
       </c>
       <c r="C231">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-185.76561919940991</v>
       </c>
       <c r="D231">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-221.38684406138461</v>
       </c>
     </row>
@@ -7706,11 +7724,11 @@
         <v>231</v>
       </c>
       <c r="C232">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-180.61495223130328</v>
       </c>
       <c r="D232">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-223.04089093815071</v>
       </c>
     </row>
@@ -7722,11 +7740,11 @@
         <v>232</v>
       </c>
       <c r="C233">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-176.0791819431382</v>
       </c>
       <c r="D233">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-225.37107553152254</v>
       </c>
     </row>
@@ -7738,11 +7756,11 @@
         <v>233</v>
       </c>
       <c r="C234">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-172.72091164463785</v>
       </c>
       <c r="D234">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-229.20839138357303</v>
       </c>
     </row>
@@ -7754,11 +7772,11 @@
         <v>234</v>
       </c>
       <c r="C235">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-167.51879690335488</v>
       </c>
       <c r="D235">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-230.56984339685999</v>
       </c>
     </row>
@@ -7770,11 +7788,11 @@
         <v>235</v>
       </c>
       <c r="C236">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-164.61643723275031</v>
       </c>
       <c r="D236">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-235.09663671094057</v>
       </c>
     </row>
@@ -7786,11 +7804,11 @@
         <v>236</v>
       </c>
       <c r="C237">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-162.1659420065167</v>
       </c>
       <c r="D237">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-240.42089604096202</v>
       </c>
     </row>
@@ -7802,11 +7820,11 @@
         <v>237</v>
       </c>
       <c r="C238">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-136.70439778877176</v>
       </c>
       <c r="D238">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-210.50631255430145</v>
       </c>
     </row>
@@ -7818,11 +7836,11 @@
         <v>238</v>
       </c>
       <c r="C239">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-131.94989679406805</v>
       </c>
       <c r="D239">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-211.16397594295006</v>
       </c>
     </row>
@@ -7834,11 +7852,11 @@
         <v>239</v>
       </c>
       <c r="C240">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-129.27455680242369</v>
       </c>
       <c r="D240">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-215.14899247623015</v>
       </c>
     </row>
@@ -7850,11 +7868,11 @@
         <v>240</v>
       </c>
       <c r="C241">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-130.00000000000011</v>
       </c>
       <c r="D241">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-225.16660498395399</v>
       </c>
     </row>
@@ -7866,11 +7884,11 @@
         <v>241</v>
       </c>
       <c r="C242">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-128.47454936527927</v>
       </c>
       <c r="D242">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-231.77422239193993</v>
       </c>
     </row>
@@ -7882,11 +7900,11 @@
         <v>242</v>
       </c>
       <c r="C243">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>0.46947156278589075</v>
       </c>
       <c r="D243">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>0.88294759285892699</v>
       </c>
     </row>
@@ -7898,11 +7916,11 @@
         <v>243</v>
       </c>
       <c r="C244">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>0.45399049973954692</v>
       </c>
       <c r="D244">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>0.89100652418836779</v>
       </c>
     </row>
@@ -7914,11 +7932,11 @@
         <v>244</v>
       </c>
       <c r="C245">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>0.43837114678907774</v>
       </c>
       <c r="D245">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>0.89879404629916682</v>
       </c>
     </row>
@@ -7930,11 +7948,11 @@
         <v>245</v>
       </c>
       <c r="C246">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>0.42261826174069994</v>
       </c>
       <c r="D246">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>0.90630778703664971</v>
       </c>
     </row>
@@ -7946,11 +7964,11 @@
         <v>246</v>
       </c>
       <c r="C247">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-216.38389411632565</v>
       </c>
       <c r="D247">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-486.00618346586373</v>
       </c>
     </row>
@@ -7962,11 +7980,11 @@
         <v>247</v>
       </c>
       <c r="C248">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-204.74311132837948</v>
       </c>
       <c r="D248">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-482.34454320907872</v>
       </c>
     </row>
@@ -7978,11 +7996,11 @@
         <v>248</v>
       </c>
       <c r="C249">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-193.29700220261074</v>
       </c>
       <c r="D249">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-478.42686895646227</v>
       </c>
     </row>
@@ -7994,11 +8012,11 @@
         <v>249</v>
       </c>
       <c r="C250">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-182.05091836901275</v>
       </c>
       <c r="D250">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-474.25885666057843</v>
       </c>
     </row>
@@ -8010,11 +8028,11 @@
         <v>250</v>
       </c>
       <c r="C251">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-171.69411194948603</v>
       </c>
       <c r="D251">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-471.72569563452589</v>
       </c>
     </row>
@@ -8026,11 +8044,11 @@
         <v>251</v>
       </c>
       <c r="C252">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-161.15623645629253</v>
       </c>
       <c r="D252">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-468.03169492166182</v>
       </c>
     </row>
@@ -8042,11 +8060,11 @@
         <v>252</v>
       </c>
       <c r="C253">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-150.80029325497441</v>
       </c>
       <c r="D253">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-464.11557995203492</v>
       </c>
     </row>
@@ -8058,11 +8076,11 @@
         <v>253</v>
       </c>
       <c r="C254">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-140.92316167635929</v>
       </c>
       <c r="D254">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-460.93889237418301</v>
       </c>
     </row>
@@ -8074,11 +8092,11 @@
         <v>254</v>
       </c>
       <c r="C255">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-131.47901872470848</v>
       </c>
       <c r="D255">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-458.52182896257818</v>
       </c>
     </row>
@@ -8090,11 +8108,11 @@
         <v>255</v>
       </c>
       <c r="C256">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-121.90377024328721</v>
       </c>
       <c r="D256">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-454.95106418215119</v>
       </c>
     </row>
@@ -8106,11 +8124,11 @@
         <v>256</v>
       </c>
       <c r="C257">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-112.73560334944519</v>
       </c>
       <c r="D257">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-452.15780844461437</v>
       </c>
     </row>
@@ -8122,11 +8140,11 @@
         <v>257</v>
       </c>
       <c r="C258">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-103.70243605252188</v>
       </c>
       <c r="D258">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-449.18459986599339</v>
       </c>
     </row>
@@ -8138,11 +8156,11 @@
         <v>258</v>
       </c>
       <c r="C259">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-94.807731012898458</v>
       </c>
       <c r="D259">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-446.03530593461534</v>
       </c>
     </row>
@@ -8154,11 +8172,11 @@
         <v>259</v>
       </c>
       <c r="C260">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-86.054856914822011</v>
       </c>
       <c r="D260">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-442.7138597348964</v>
       </c>
     </row>
@@ -8170,11 +8188,11 @@
         <v>260</v>
       </c>
       <c r="C261">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-77.620735417117857</v>
       </c>
       <c r="D261">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-440.20906559645698</v>
       </c>
     </row>
@@ -8186,11 +8204,11 @@
         <v>261</v>
       </c>
       <c r="C262">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-69.144033547782115</v>
       </c>
       <c r="D262">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-436.55824654305087</v>
       </c>
     </row>
@@ -8202,11 +8220,11 @@
         <v>262</v>
       </c>
       <c r="C263">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-61.096991321468508</v>
       </c>
       <c r="D263">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-434.72768217754941</v>
       </c>
     </row>
@@ -8218,11 +8236,11 @@
         <v>263</v>
       </c>
       <c r="C264">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-53.013164381239022</v>
       </c>
       <c r="D264">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-431.75757596397511</v>
       </c>
     </row>
@@ -8234,11 +8252,11 @@
         <v>264</v>
       </c>
       <c r="C265">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-45.0517676683586</v>
       </c>
       <c r="D265">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-428.63893690372583</v>
       </c>
     </row>
@@ -8250,11 +8268,11 @@
         <v>265</v>
       </c>
       <c r="C266">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-37.302657895997733</v>
       </c>
       <c r="D266">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-426.37133078326707</v>
       </c>
     </row>
@@ -8266,11 +8284,11 @@
         <v>266</v>
       </c>
       <c r="C267">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-29.646501341253373</v>
       </c>
       <c r="D267">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-423.9647213604253</v>
       </c>
     </row>
@@ -8282,11 +8300,11 @@
         <v>267</v>
       </c>
       <c r="C268">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-22.085773534522499</v>
       </c>
       <c r="D268">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-421.42166366643016</v>
       </c>
     </row>
@@ -8298,11 +8316,11 @@
         <v>268</v>
       </c>
       <c r="C269">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-14.622889118348191</v>
       </c>
       <c r="D269">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-418.74475652100108</v>
       </c>
     </row>
@@ -8314,11 +8332,11 @@
         <v>269</v>
       </c>
       <c r="C270">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-7.2602010779099349</v>
       </c>
       <c r="D270">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-415.93664118505876</v>
       </c>
     </row>
@@ -8330,11 +8348,11 @@
         <v>270</v>
       </c>
       <c r="C271">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>-7.6081719049825303E-14</v>
       </c>
       <c r="D271">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-414</v>
       </c>
     </row>
@@ -8346,11 +8364,11 @@
         <v>271</v>
       </c>
       <c r="C272">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>7.1729390457233668</v>
       </c>
       <c r="D272">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-410.9374027092768</v>
       </c>
     </row>
@@ -8362,11 +8380,11 @@
         <v>272</v>
       </c>
       <c r="C273">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>14.273894151323024</v>
       </c>
       <c r="D273">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-408.75084825081018</v>
       </c>
     </row>
@@ -8378,11 +8396,11 @@
         <v>273</v>
       </c>
       <c r="C274">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>21.300734190878185</v>
       </c>
       <c r="D274">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-406.44222064511155</v>
       </c>
     </row>
@@ -8394,11 +8412,11 @@
         <v>274</v>
       </c>
       <c r="C275">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>28.18161539262659</v>
       </c>
       <c r="D275">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-403.01587630496903</v>
       </c>
     </row>
@@ -8410,11 +8428,11 @@
         <v>275</v>
       </c>
       <c r="C276">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>35.123764327306127</v>
       </c>
       <c r="D276">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-401.46646333097345</v>
       </c>
     </row>
@@ -8426,11 +8444,11 @@
         <v>276</v>
       </c>
       <c r="C277">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>41.915913770328849</v>
       </c>
       <c r="D277">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-398.80328004267761</v>
       </c>
     </row>
@@ -8442,11 +8460,11 @@
         <v>277</v>
       </c>
       <c r="C278">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>48.625868018653925</v>
       </c>
       <c r="D278">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-396.02591450488745</v>
       </c>
     </row>
@@ -8458,11 +8476,11 @@
         <v>278</v>
       </c>
       <c r="C279">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>55.390894182106052</v>
       </c>
       <c r="D279">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-394.12669135914501</v>
       </c>
     </row>
@@ -8474,11 +8492,11 @@
         <v>279</v>
       </c>
       <c r="C280">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>61.948048155931346</v>
       </c>
       <c r="D280">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-391.12458287567455</v>
       </c>
     </row>
@@ -8490,11 +8508,11 @@
         <v>280</v>
       </c>
       <c r="C281">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>68.76467835610427</v>
       </c>
       <c r="D281">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-389.98387019283444</v>
       </c>
     </row>
@@ -8506,11 +8524,11 @@
         <v>281</v>
       </c>
       <c r="C282">
-        <f t="shared" ref="C282:C345" si="20">A282*COS(B282*PI()/180)</f>
+        <f t="shared" ref="C282:C345" si="16">A282*COS(B282*PI()/180)</f>
         <v>75.178744178358428</v>
       </c>
       <c r="D282">
-        <f t="shared" ref="D282:D345" si="21">A282*SIN(B282*PI()/180)</f>
+        <f t="shared" ref="D282:D345" si="17">A282*SIN(B282*PI()/180)</f>
         <v>-386.76111027837965</v>
       </c>
     </row>
@@ -8522,11 +8540,11 @@
         <v>282</v>
       </c>
       <c r="C283">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>81.709294491379111</v>
       </c>
       <c r="D283">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-384.41200708838568</v>
       </c>
     </row>
@@ -8538,11 +8556,11 @@
         <v>283</v>
       </c>
       <c r="C284">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>87.955862248451183</v>
       </c>
       <c r="D284">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-380.97869533102698</v>
       </c>
     </row>
@@ -8554,11 +8572,11 @@
         <v>284</v>
       </c>
       <c r="C285">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>94.3495392838703</v>
       </c>
       <c r="D285">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-378.41533324763867</v>
       </c>
     </row>
@@ -8570,11 +8588,11 @@
         <v>285</v>
       </c>
       <c r="C286">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>100.93942758998324</v>
       </c>
       <c r="D286">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-376.71107225273659</v>
       </c>
     </row>
@@ -8586,11 +8604,11 @@
         <v>286</v>
       </c>
       <c r="C287">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>107.49856876862977</v>
       </c>
       <c r="D287">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-374.89206141594434</v>
       </c>
     </row>
@@ -8602,11 +8620,11 @@
         <v>287</v>
       </c>
       <c r="C288">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>114.31733654659006</v>
       </c>
       <c r="D288">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-373.91515958154685</v>
       </c>
     </row>
@@ -8618,11 +8636,11 @@
         <v>288</v>
       </c>
       <c r="C289">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>120.51662780622942</v>
       </c>
       <c r="D289">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-370.91204135510992</v>
       </c>
     </row>
@@ -8634,11 +8652,11 @@
         <v>289</v>
       </c>
       <c r="C290">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>126.97158023829095</v>
       </c>
       <c r="D290">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-368.75224448373359</v>
       </c>
     </row>
@@ -8650,11 +8668,11 @@
         <v>290</v>
       </c>
       <c r="C291">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>133.72987604033625</v>
       </c>
       <c r="D291">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-367.41981472729026</v>
       </c>
     </row>
@@ -8666,11 +8684,11 @@
         <v>291</v>
       </c>
       <c r="C292">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>140.12186827221211</v>
       </c>
       <c r="D292">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-365.02994676040601</v>
       </c>
     </row>
@@ -8682,11 +8700,11 @@
         <v>292</v>
       </c>
       <c r="C293">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>146.84578461903749</v>
       </c>
       <c r="D293">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-363.45607099018065</v>
       </c>
     </row>
@@ -8698,11 +8716,11 @@
         <v>293</v>
       </c>
       <c r="C294">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>153.55733349628449</v>
       </c>
       <c r="D294">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-361.75840740680911</v>
       </c>
     </row>
@@ -8714,11 +8732,11 @@
         <v>294</v>
       </c>
       <c r="C295">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>160.2542373718654</v>
       </c>
       <c r="D295">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-359.9369103111847</v>
       </c>
     </row>
@@ -8730,11 +8748,11 @@
         <v>295</v>
       </c>
       <c r="C296">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>166.93421338757634</v>
       </c>
       <c r="D296">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-357.99157587947673</v>
       </c>
     </row>
@@ -8746,11 +8764,11 @@
         <v>296</v>
       </c>
       <c r="C297">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>173.59497412847466</v>
       </c>
       <c r="D297">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-355.92244233447013</v>
       </c>
     </row>
@@ -8762,11 +8780,11 @@
         <v>297</v>
       </c>
       <c r="C298">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>180.2342283966</v>
       </c>
       <c r="D298">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-353.72959010278208</v>
       </c>
     </row>
@@ -8778,11 +8796,11 @@
         <v>298</v>
       </c>
       <c r="C299">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>118.77630538483028</v>
       </c>
       <c r="D299">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-223.38574099330856</v>
       </c>
     </row>
@@ -8794,11 +8812,11 @@
         <v>299</v>
       </c>
       <c r="C300">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>116.8391184793671</v>
       </c>
       <c r="D300">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-210.78334942059445</v>
       </c>
     </row>
@@ -8810,11 +8828,11 @@
         <v>300</v>
       </c>
       <c r="C301">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>120.50000000000003</v>
       </c>
       <c r="D301">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-208.7121223120497</v>
       </c>
     </row>
@@ -8826,11 +8844,11 @@
         <v>301</v>
       </c>
       <c r="C302">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>124.12417605332305</v>
       </c>
       <c r="D302">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-206.57731946920907</v>
       </c>
     </row>
@@ -8842,11 +8860,11 @@
         <v>302</v>
       </c>
       <c r="C303">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>127.18062341596912</v>
       </c>
       <c r="D303">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-203.5315430775423</v>
       </c>
     </row>
@@ -8858,11 +8876,11 @@
         <v>303</v>
       </c>
       <c r="C304">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>129.62409033357633</v>
       </c>
       <c r="D304">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-199.60359517101097</v>
       </c>
     </row>
@@ -8874,11 +8892,11 @@
         <v>304</v>
       </c>
       <c r="C305">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>133.0879110260376</v>
       </c>
       <c r="D305">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-197.31094226810001</v>
       </c>
     </row>
@@ -8890,11 +8908,11 @@
         <v>305</v>
       </c>
       <c r="C306">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>137.0847682879</v>
       </c>
       <c r="D306">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-195.77733858506903</v>
       </c>
     </row>
@@ -8906,11 +8924,11 @@
         <v>306</v>
       </c>
       <c r="C307">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>141.65624580248598</v>
       </c>
       <c r="D307">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-194.97309564436236</v>
       </c>
     </row>
@@ -8922,11 +8940,11 @@
         <v>307</v>
       </c>
       <c r="C308">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>146.84286564909971</v>
       </c>
       <c r="D308">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-194.86706445153951</v>
       </c>
     </row>
@@ -8938,11 +8956,11 @@
         <v>308</v>
       </c>
       <c r="C309">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>152.06838440543766</v>
       </c>
       <c r="D309">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-194.63865614086029</v>
       </c>
     </row>
@@ -8954,11 +8972,11 @@
         <v>309</v>
       </c>
       <c r="C310">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>159.84737932665874</v>
       </c>
       <c r="D310">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-197.39507421007059</v>
       </c>
     </row>
@@ -8970,11 +8988,11 @@
         <v>310</v>
       </c>
       <c r="C311">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>-0.64278760968653925</v>
       </c>
       <c r="D311">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>0.76604444311897812</v>
       </c>
     </row>
@@ -8986,11 +9004,11 @@
         <v>311</v>
       </c>
       <c r="C312">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>-0.65605902899050705</v>
       </c>
       <c r="D312">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>0.75470958022277224</v>
       </c>
     </row>
@@ -9002,11 +9020,11 @@
         <v>312</v>
       </c>
       <c r="C313">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>-0.66913060635885779</v>
       </c>
       <c r="D313">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>0.74314482547739458</v>
       </c>
     </row>
@@ -9018,11 +9036,11 @@
         <v>313</v>
       </c>
       <c r="C314">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>298.71528170737412</v>
       </c>
       <c r="D314">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-320.33292130919688</v>
       </c>
     </row>
@@ -9034,11 +9052,11 @@
         <v>314</v>
       </c>
       <c r="C315">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>305.64968300195852</v>
       </c>
       <c r="D315">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-316.50951214900675</v>
       </c>
     </row>
@@ -9050,11 +9068,11 @@
         <v>315</v>
       </c>
       <c r="C316">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>313.95541084682702</v>
       </c>
       <c r="D316">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-313.95541084682719</v>
       </c>
     </row>
@@ -9066,11 +9084,11 @@
         <v>316</v>
       </c>
       <c r="C317">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>322.26423055171557</v>
       </c>
       <c r="D317">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-311.20694996563094</v>
       </c>
     </row>
@@ -9082,11 +9100,11 @@
         <v>317</v>
       </c>
       <c r="C318">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>330.57187313186517</v>
       </c>
       <c r="D318">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-308.2632587482492</v>
       </c>
     </row>
@@ -9098,11 +9116,11 @@
         <v>318</v>
       </c>
       <c r="C319">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>339.61718524316916</v>
       </c>
       <c r="D319">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-305.79268710599814</v>
       </c>
     </row>
@@ -9114,11 +9132,11 @@
         <v>319</v>
       </c>
       <c r="C320">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>348.67582606292063</v>
       </c>
       <c r="D320">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-303.0992713936144</v>
       </c>
     </row>
@@ -9130,11 +9148,11 @@
         <v>320</v>
       </c>
       <c r="C321">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>357.74275493656262</v>
       </c>
       <c r="D321">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-300.18181372361397</v>
       </c>
     </row>
@@ -9146,11 +9164,11 @@
         <v>321</v>
       </c>
       <c r="C322">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>367.5900397691471</v>
       </c>
       <c r="D322">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-297.66854496657328</v>
       </c>
     </row>
@@ -9162,11 +9180,11 @@
         <v>322</v>
       </c>
       <c r="C323">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>376.66914022401289</v>
       </c>
       <c r="D323">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-294.28618520566494</v>
       </c>
     </row>
@@ -9178,11 +9196,11 @@
         <v>323</v>
       </c>
       <c r="C324">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>386.53958686288973</v>
       </c>
       <c r="D324">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-291.27847120559136</v>
       </c>
     </row>
@@ -9194,11 +9212,11 @@
         <v>324</v>
       </c>
       <c r="C325">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>396.41832724372421</v>
       </c>
       <c r="D325">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-288.01477362331195</v>
       </c>
     </row>
@@ -9210,11 +9228,11 @@
         <v>325</v>
       </c>
       <c r="C326">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>406.29941396733983</v>
       </c>
       <c r="D326">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-284.49391243011905</v>
       </c>
     </row>
@@ -9226,11 +9244,11 @@
         <v>326</v>
       </c>
       <c r="C327">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>417.00589899518582</v>
       </c>
       <c r="D327">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-281.27403044578591</v>
       </c>
     </row>
@@ -9242,11 +9260,11 @@
         <v>327</v>
       </c>
       <c r="C328">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>427.72198965216626</v>
       </c>
       <c r="D328">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-277.76590785766376</v>
       </c>
     </row>
@@ -9258,11 +9276,11 @@
         <v>328</v>
       </c>
       <c r="C329">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>438.44086571287193</v>
       </c>
       <c r="D329">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-273.96825960856739</v>
       </c>
     </row>
@@ -9274,11 +9292,11 @@
         <v>329</v>
       </c>
       <c r="C330">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>450.01283286860888</v>
       </c>
       <c r="D330">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-270.3949893277786</v>
       </c>
     </row>
@@ -9290,11 +9308,11 @@
         <v>330</v>
       </c>
       <c r="C331">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>461.59154021710566</v>
       </c>
       <c r="D331">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-266.50000000000023</v>
       </c>
     </row>
@@ -9306,11 +9324,11 @@
         <v>331</v>
       </c>
       <c r="C332">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>473.16926156241317</v>
       </c>
       <c r="D332">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-262.28200455326828</v>
       </c>
     </row>
@@ -9322,11 +9340,11 @@
         <v>332</v>
       </c>
       <c r="C333">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>484.73822847955086</v>
       </c>
       <c r="D333">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-257.73988796945406</v>
       </c>
     </row>
@@ -9338,11 +9356,11 @@
         <v>333</v>
       </c>
       <c r="C334">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>498.0726470212976</v>
       </c>
       <c r="D334">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-253.78068935440675</v>
       </c>
     </row>
@@ -9354,11 +9372,11 @@
         <v>334</v>
       </c>
       <c r="C335">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>509.61622425162778</v>
       </c>
       <c r="D335">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-248.55644022940666</v>
       </c>
     </row>
@@ -9370,11 +9388,11 @@
         <v>335</v>
       </c>
       <c r="C336">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>522.93959312014692</v>
       </c>
       <c r="D336">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-243.8507370243839</v>
       </c>
     </row>
@@ -9386,11 +9404,11 @@
         <v>336</v>
       </c>
       <c r="C337">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>536.25118363620675</v>
       </c>
       <c r="D337">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-238.75440948549468</v>
       </c>
     </row>
@@ -9402,11 +9420,11 @@
         <v>337</v>
       </c>
       <c r="C338">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>548.62089265765417</v>
       </c>
       <c r="D338">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-232.87575257960773</v>
       </c>
     </row>
@@ -9418,11 +9436,11 @@
         <v>338</v>
       </c>
       <c r="C339">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>562.80059972203992</v>
       </c>
       <c r="D339">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-227.38620220345879</v>
       </c>
     </row>
@@ -9434,11 +9452,11 @@
         <v>339</v>
       </c>
       <c r="C340">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>554.54677333933773</v>
       </c>
       <c r="D340">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-212.87056202990865</v>
       </c>
     </row>
@@ -9450,11 +9468,11 @@
         <v>340</v>
       </c>
       <c r="C341">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>549.7201831597564</v>
       </c>
       <c r="D341">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-200.08178384551613</v>
       </c>
     </row>
@@ -9466,11 +9484,11 @@
         <v>341</v>
       </c>
       <c r="C342">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>544.61869954520625</v>
       </c>
       <c r="D342">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-187.52725696732273</v>
       </c>
     </row>
@@ -9482,11 +9500,11 @@
         <v>342</v>
       </c>
       <c r="C343">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>540.20010125564716</v>
       </c>
       <c r="D343">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-175.52165280497024</v>
       </c>
     </row>
@@ -9498,11 +9516,11 @@
         <v>343</v>
       </c>
       <c r="C344">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>535.53066333929996</v>
       </c>
       <c r="D344">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-163.72815464473231</v>
       </c>
     </row>
@@ -9514,11 +9532,11 @@
         <v>344</v>
       </c>
       <c r="C345">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>532.53897954982858</v>
       </c>
       <c r="D345">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>-152.70309512261787</v>
       </c>
     </row>
@@ -9530,11 +9548,11 @@
         <v>345</v>
       </c>
       <c r="C346">
-        <f t="shared" ref="C346:C360" si="22">A346*COS(B346*PI()/180)</f>
+        <f t="shared" ref="C346:C360" si="18">A346*COS(B346*PI()/180)</f>
         <v>527.39550115383133</v>
       </c>
       <c r="D346">
-        <f t="shared" ref="D346:D360" si="23">A346*SIN(B346*PI()/180)</f>
+        <f t="shared" ref="D346:D360" si="19">A346*SIN(B346*PI()/180)</f>
         <v>-141.31519862597628</v>
       </c>
     </row>
@@ -9546,11 +9564,11 @@
         <v>346</v>
       </c>
       <c r="C347">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>523.95969218903815</v>
       </c>
       <c r="D347">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>-130.63782362382065</v>
       </c>
     </row>
@@ -9562,11 +9580,11 @@
         <v>347</v>
       </c>
       <c r="C348">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>519.33924453053032</v>
       </c>
       <c r="D348">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>-119.89891196528022</v>
       </c>
     </row>
@@ -9578,11 +9596,11 @@
         <v>348</v>
       </c>
       <c r="C349">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>515.4837855867155</v>
       </c>
       <c r="D349">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>-109.56946106095945</v>
       </c>
     </row>
@@ -9594,11 +9612,11 @@
         <v>349</v>
       </c>
       <c r="C350">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>511.42776257623291</v>
       </c>
       <c r="D350">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>-99.411486591179766</v>
       </c>
     </row>
@@ -9610,11 +9628,11 @@
         <v>350</v>
       </c>
       <c r="C351">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>508.16080055429927</v>
       </c>
       <c r="D351">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>-89.602459676136533</v>
       </c>
     </row>
@@ -9626,11 +9644,11 @@
         <v>351</v>
       </c>
       <c r="C352">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>-0.98768834059513766</v>
       </c>
       <c r="D352">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>0.15643446504023112</v>
       </c>
     </row>
@@ -9642,11 +9660,11 @@
         <v>352</v>
       </c>
       <c r="C353">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>502.06591085197613</v>
       </c>
       <c r="D353">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>-70.560762186753408</v>
       </c>
     </row>
@@ -9658,11 +9676,11 @@
         <v>353</v>
       </c>
       <c r="C354">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>497.26562197230231</v>
       </c>
       <c r="D354">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>-61.056541045979202</v>
       </c>
     </row>
@@ -9674,11 +9692,11 @@
         <v>354</v>
       </c>
       <c r="C355">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>493.28286010266356</v>
       </c>
       <c r="D355">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>-51.846117780756096</v>
       </c>
     </row>
@@ -9690,11 +9708,11 @@
         <v>355</v>
       </c>
       <c r="C356">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>490.12779146113883</v>
       </c>
       <c r="D356">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>-42.880625431847889</v>
       </c>
     </row>
@@ -9706,11 +9724,11 @@
         <v>356</v>
       </c>
       <c r="C357">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>486.81125652679424</v>
       </c>
       <c r="D357">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>-34.041159187132884</v>
       </c>
     </row>
@@ -9722,11 +9740,11 @@
         <v>357</v>
       </c>
       <c r="C358">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>484.33532435596828</v>
       </c>
       <c r="D358">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>-25.38293877782802</v>
       </c>
     </row>
@@ -9738,11 +9756,11 @@
         <v>358</v>
       </c>
       <c r="C359">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>480.70698779618505</v>
       </c>
       <c r="D359">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>-16.786657913902896</v>
       </c>
     </row>
@@ -9754,11 +9772,11 @@
         <v>359</v>
       </c>
       <c r="C360">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>477.92719828475504</v>
       </c>
       <c r="D360">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>-8.3422502770219662</v>
       </c>
     </row>

</xml_diff>